<commit_message>
Added new SIA options
"Section":  "sia",
"Item":  "ca_repository_directory_name",
"Item":  "ca_repository_https",
"Item":  "ca_repository_ldaps",
"Item":  "ca_repository_http_p7c",
"Item":  "time_stamping_present",
</commit_message>
<xml_diff>
--- a/docs/profile-config.xlsx
+++ b/docs/profile-config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="314">
   <si>
     <t>BOOL</t>
   </si>
@@ -945,6 +945,27 @@
   </si>
   <si>
     <t>require use of p7c</t>
+  </si>
+  <si>
+    <t>ca_repository_directory_name</t>
+  </si>
+  <si>
+    <t>ca_repository_https</t>
+  </si>
+  <si>
+    <t>ca_repository_ldaps</t>
+  </si>
+  <si>
+    <t>ca_repository_http_p7c</t>
+  </si>
+  <si>
+    <t>time_stamping_present</t>
+  </si>
+  <si>
+    <t>can use tls for ldap sia?</t>
+  </si>
+  <si>
+    <t>can use tls for http sia?</t>
   </si>
 </sst>
 </file>
@@ -1364,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I203"/>
+  <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:XFD110"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3967,18 +3988,15 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>249</v>
+      <c r="A119" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>179</v>
+        <v>307</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="E119" s="3" t="s">
         <v>2</v>
       </c>
@@ -3990,14 +4008,14 @@
       </c>
     </row>
     <row r="120" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>249</v>
+      <c r="A120" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>180</v>
+        <v>308</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>21</v>
+        <v>279</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>2</v>
@@ -4008,42 +4026,43 @@
       <c r="G120" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H120" s="1" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="121" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F121" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G121" s="8" t="s">
-        <v>82</v>
+      <c r="A121" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>250</v>
+      <c r="A122" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>179</v>
+        <v>310</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="E122" s="3" t="s">
         <v>2</v>
       </c>
@@ -4053,13 +4072,16 @@
       <c r="G122" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H122" s="1" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="123" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>250</v>
+      <c r="A123" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>180</v>
+        <v>311</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>21</v>
@@ -4076,36 +4098,36 @@
     </row>
     <row r="124" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>214</v>
+        <v>179</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H124" s="1" t="s">
-        <v>284</v>
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>2</v>
@@ -4119,33 +4141,38 @@
     </row>
     <row r="126" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F126" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>18</v>
+        <v>249</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G126" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>2</v>
@@ -4159,10 +4186,10 @@
     </row>
     <row r="128" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>21</v>
@@ -4179,22 +4206,22 @@
     </row>
     <row r="129" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>21</v>
+        <v>214</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>18</v>
+        <v>263</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4202,10 +4229,13 @@
         <v>251</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>2</v>
@@ -4222,7 +4252,7 @@
         <v>251</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>21</v>
@@ -4242,7 +4272,7 @@
         <v>251</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>21</v>
@@ -4262,7 +4292,7 @@
         <v>251</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>21</v>
@@ -4282,7 +4312,7 @@
         <v>251</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>21</v>
@@ -4302,7 +4332,7 @@
         <v>251</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>21</v>
@@ -4322,13 +4352,10 @@
         <v>251</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>2</v>
@@ -4345,13 +4372,10 @@
         <v>251</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>2</v>
@@ -4368,7 +4392,7 @@
         <v>251</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>21</v>
@@ -4381,26 +4405,17 @@
       </c>
       <c r="G138" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="H138" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I138" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>2</v>
@@ -4414,10 +4429,10 @@
     </row>
     <row r="140" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>21</v>
@@ -4434,13 +4449,16 @@
     </row>
     <row r="141" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>2</v>
@@ -4454,13 +4472,16 @@
     </row>
     <row r="142" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>2</v>
@@ -4474,10 +4495,10 @@
     </row>
     <row r="143" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>21</v>
@@ -4490,6 +4511,12 @@
       </c>
       <c r="G143" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4497,10 +4524,13 @@
         <v>252</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="E144" s="3" t="s">
         <v>2</v>
@@ -4517,7 +4547,7 @@
         <v>252</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>21</v>
@@ -4537,7 +4567,7 @@
         <v>252</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>21</v>
@@ -4557,7 +4587,7 @@
         <v>252</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>21</v>
@@ -4577,7 +4607,7 @@
         <v>252</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>21</v>
@@ -4597,7 +4627,7 @@
         <v>252</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>21</v>
@@ -4617,13 +4647,10 @@
         <v>252</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E150" s="3" t="s">
         <v>2</v>
@@ -4640,13 +4667,10 @@
         <v>252</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>2</v>
@@ -4663,7 +4687,7 @@
         <v>252</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>21</v>
@@ -4676,26 +4700,17 @@
       </c>
       <c r="G152" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="H152" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I152" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E153" s="3" t="s">
         <v>2</v>
@@ -4709,10 +4724,10 @@
     </row>
     <row r="154" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>21</v>
@@ -4729,16 +4744,16 @@
     </row>
     <row r="155" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="E155" s="3" t="s">
         <v>2</v>
@@ -4752,13 +4767,16 @@
     </row>
     <row r="156" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>2</v>
@@ -4772,10 +4790,10 @@
     </row>
     <row r="157" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>21</v>
@@ -4788,17 +4806,26 @@
       </c>
       <c r="G157" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I157" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>2</v>
@@ -4812,10 +4839,10 @@
     </row>
     <row r="159" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>21</v>
@@ -4824,15 +4851,15 @@
         <v>2</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>179</v>
@@ -4841,7 +4868,7 @@
         <v>21</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>2</v>
@@ -4853,9 +4880,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>180</v>
@@ -4873,136 +4900,136 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B165" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C162" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F162" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
+      <c r="C167" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C163" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F163" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G163" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F164" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G165" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E167" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F167" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G167" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="C168" s="1" t="s">
         <v>21</v>
       </c>
@@ -5016,260 +5043,251 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>256</v>
       </c>
       <c r="B169" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F169" s="3" t="s">
+      <c r="C174" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F174" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G169" s="1" t="s">
+      <c r="G174" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
+    <row r="175" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B175" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C170" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D170" s="1" t="s">
+      <c r="C175" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D175" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E170" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F170" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+      <c r="E175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B176" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C171" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G171" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="1" t="s">
+      <c r="C176" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D172" s="1" t="s">
+      <c r="C177" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D177" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E172" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F172" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G172" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="1" t="s">
+      <c r="E177" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B178" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E173" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F173" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G173" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="1" t="s">
+      <c r="C178" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B179" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C174" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D174" s="1" t="s">
+      <c r="C179" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D179" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E174" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F174" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H174" s="1" t="s">
+      <c r="E179" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H179" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
+    <row r="180" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B180" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C175" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E175" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F175" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G175" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E176" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F176" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G176" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F177" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G177" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F178" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G178" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F179" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G179" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="C180" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D180" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E180" s="3" t="s">
         <v>2</v>
       </c>
@@ -5280,18 +5298,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>2</v>
@@ -5303,19 +5321,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D182" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E182" s="3" t="s">
         <v>2</v>
       </c>
@@ -5326,18 +5341,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>2</v>
@@ -5349,18 +5364,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>2</v>
@@ -5372,18 +5387,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>2</v>
@@ -5395,18 +5410,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>2</v>
@@ -5418,18 +5433,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>2</v>
@@ -5441,18 +5456,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D188" s="9" t="s">
-        <v>57</v>
+      <c r="D188" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>2</v>
@@ -5464,18 +5479,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D189" s="9" t="s">
-        <v>58</v>
+      <c r="D189" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>2</v>
@@ -5487,18 +5502,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D190" s="10" t="s">
-        <v>60</v>
+      <c r="D190" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>2</v>
@@ -5510,18 +5525,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D191" s="9" t="s">
-        <v>61</v>
+      <c r="D191" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>2</v>
@@ -5533,18 +5548,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D192" s="9" t="s">
-        <v>41</v>
+      <c r="D192" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>2</v>
@@ -5561,13 +5576,13 @@
         <v>260</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>2</v>
@@ -5584,13 +5599,13 @@
         <v>260</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>2</v>
@@ -5607,13 +5622,13 @@
         <v>260</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>297</v>
+        <v>231</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D195" s="9" t="s">
-        <v>298</v>
+      <c r="D195" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>2</v>
@@ -5630,13 +5645,13 @@
         <v>260</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>299</v>
+        <v>232</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>300</v>
+        <v>61</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>2</v>
@@ -5653,13 +5668,13 @@
         <v>260</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>301</v>
+        <v>233</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>302</v>
+        <v>41</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>2</v>
@@ -5676,13 +5691,13 @@
         <v>260</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>303</v>
+        <v>234</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>304</v>
+        <v>62</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>2</v>
@@ -5699,11 +5714,14 @@
         <v>260</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D199" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E199" s="3" t="s">
         <v>2</v>
       </c>
@@ -5712,23 +5730,20 @@
       </c>
       <c r="G199" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="H199" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D200" s="1" t="s">
-        <v>114</v>
+      <c r="D200" s="9" t="s">
+        <v>298</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>2</v>
@@ -5742,13 +5757,16 @@
     </row>
     <row r="201" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>180</v>
+        <v>299</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D201" s="9" t="s">
+        <v>300</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>2</v>
@@ -5762,41 +5780,153 @@
     </row>
     <row r="202" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D202" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D203" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="B207" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C202" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E202" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F202" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G202" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A203" s="1" t="s">
+      <c r="C207" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B203" s="2" t="s">
+      <c r="B208" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C203" s="1" t="s">
+      <c r="C208" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E203" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F203" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G203" s="1" t="s">
+      <c r="E208" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G208" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>